<commit_message>
added to be albe to play woth more players
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\programering\C#\campus mölndal\BlackJack_TDD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D50B37-2C34-44B0-89FB-D04F18E7CB94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Blad1" sheetId="1" r:id="rId4"/>
+    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>Scenario</t>
   </si>
@@ -206,31 +215,29 @@
   </si>
   <si>
     <t xml:space="preserve">bet: 400 hand.count = 2 splithand.count = 2 </t>
-  </si>
-  <si>
-    <t>FALSE "Cards aint equal"</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;docs-Calibri&quot;"/>
     </font>
@@ -240,11 +247,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="10">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF999999"/>
@@ -258,44 +271,524 @@
       <bottom style="thin">
         <color rgb="FF999999"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF999999"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF999999"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF999999"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF999999"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF999999"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF999999"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF999999"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF999999"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF999999"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF999999"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF999999"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF999999"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF999999"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF999999"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF999999"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF999999"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF999999"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF999999"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF999999"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF999999"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF999999"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF999999"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF999999"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF999999"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF999999"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF999999"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF999999"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF999999"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF999999"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C365CD27-DED0-4BCB-8F9C-3BA7354AF366}" name="Table1" displayName="Table1" ref="A1:H26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+  <autoFilter ref="A1:H26" xr:uid="{E93033CE-BFE7-44D2-8C5D-02FF1F3EFF4A}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{0A2024A0-3362-4B6A-8F17-486E9F487152}" name="Scenario" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{01F1AA0E-73A2-4D6A-B981-6384E62C7F85}" name="Cases" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{793E7F07-D941-4914-A473-A1D4EBF03601}" name="ID" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4FD93DED-5630-472D-9939-957CC55D5DC4}" name="Steps" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{B3D21B56-6331-4C7A-9682-9E2BD94AE016}" name="Data" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{3BF138EB-AC0D-4114-B7CF-56EA3AAC9B44}" name="Expected" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{F4AB2CC1-2706-4790-ABA7-E33B1E5FFF67}" name="Actual" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{7DFD0621-A157-42ED-A951-4DD7CBFEBEC5}" name="Resualt" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -485,56 +978,59 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.13"/>
-    <col customWidth="1" min="2" max="2" width="12.88"/>
-    <col customWidth="1" min="3" max="3" width="5.25"/>
-    <col customWidth="1" min="4" max="4" width="13.63"/>
-    <col customWidth="1" min="5" max="5" width="17.38"/>
-    <col customWidth="1" min="6" max="7" width="16.25"/>
-    <col customWidth="1" min="8" max="26" width="7.63"/>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="32.125" customWidth="1"/>
+    <col min="3" max="3" width="5.25" customWidth="1"/>
+    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="17.375" customWidth="1"/>
+    <col min="6" max="7" width="16.25" customWidth="1"/>
+    <col min="8" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="26" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="33.0" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" ht="33" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -555,12 +1051,12 @@
       <c r="G2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:8" ht="30">
+      <c r="A3" s="6"/>
       <c r="B3" s="3"/>
       <c r="C3" s="1" t="s">
         <v>14</v>
@@ -577,12 +1073,12 @@
       <c r="G3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="6"/>
       <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
         <v>18</v>
@@ -599,12 +1095,12 @@
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:8" ht="42.75">
+      <c r="A5" s="6"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
@@ -621,12 +1117,12 @@
       <c r="G5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:8" ht="57">
+      <c r="A6" s="6"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
         <v>25</v>
@@ -643,12 +1139,12 @@
       <c r="G6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" ht="47.25" customHeight="1">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:8" ht="47.25" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -669,12 +1165,12 @@
       <c r="G7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3"/>
+    <row r="8" spans="1:8">
+      <c r="A8" s="6"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
         <v>33</v>
@@ -691,12 +1187,12 @@
       <c r="G8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="3"/>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
         <v>37</v>
@@ -713,12 +1209,12 @@
       <c r="G9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3"/>
+    <row r="10" spans="1:8" ht="28.5">
+      <c r="A10" s="6"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
         <v>41</v>
@@ -735,12 +1231,12 @@
       <c r="G10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="3"/>
+    <row r="11" spans="1:8" ht="42.75">
+      <c r="A11" s="6"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
         <v>44</v>
@@ -757,12 +1253,12 @@
       <c r="G11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:8" ht="57">
+      <c r="A12" s="6"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
         <v>47</v>
@@ -779,12 +1275,12 @@
       <c r="G12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:8" ht="28.5">
+      <c r="A13" s="6"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4" t="s">
         <v>51</v>
@@ -801,12 +1297,12 @@
       <c r="G13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="3"/>
+    <row r="14" spans="1:8" ht="42.75">
+      <c r="A14" s="6"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4" t="s">
         <v>55</v>
@@ -823,12 +1319,12 @@
       <c r="G14" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="3"/>
+    <row r="15" spans="1:8" ht="28.5">
+      <c r="A15" s="6"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4" t="s">
         <v>58</v>
@@ -845,12 +1341,12 @@
       <c r="G15" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="3"/>
+    <row r="16" spans="1:8" ht="57">
+      <c r="A16" s="6"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4" t="s">
         <v>61</v>
@@ -865,118 +1361,118 @@
         <v>64</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="6"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="3"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="3"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="6"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="3"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="6"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="3"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="6"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="3"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A22" s="6"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="3"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A23" s="6"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="3"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A24" s="6"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="3"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A25" s="6"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1947,9 +2443,10 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fyllt i testmetoder i Excel.
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\programering\C#\campus mölndal\BlackJack_TDD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D50B37-2C34-44B0-89FB-D04F18E7CB94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Blad1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="90">
   <si>
     <t>Scenario</t>
   </si>
@@ -215,31 +206,102 @@
   </si>
   <si>
     <t xml:space="preserve">bet: 400 hand.count = 2 splithand.count = 2 </t>
+  </si>
+  <si>
+    <t>F16</t>
+  </si>
+  <si>
+    <t>DesignTest</t>
+  </si>
+  <si>
+    <t>Testar så kortet inte är null</t>
+  </si>
+  <si>
+    <t>Assert.IsNotNull(cardDesign)</t>
+  </si>
+  <si>
+    <t>NotNull</t>
+  </si>
+  <si>
+    <t>F17</t>
+  </si>
+  <si>
+    <t>FlipCardTest</t>
+  </si>
+  <si>
+    <t>Assert.IsFals(card.isVisible)</t>
+  </si>
+  <si>
+    <t>F18</t>
+  </si>
+  <si>
+    <t>DrawCardTest1</t>
+  </si>
+  <si>
+    <t>Assert.IsNotNull(c, c.Value.ToString());</t>
+  </si>
+  <si>
+    <t>Not Null</t>
+  </si>
+  <si>
+    <t>F19</t>
+  </si>
+  <si>
+    <t>DrawCardTest2</t>
+  </si>
+  <si>
+    <t>Assert.IsNotNull(c, c.Suit.ToString());</t>
+  </si>
+  <si>
+    <t>F20</t>
+  </si>
+  <si>
+    <t>ShuffleDeck</t>
+  </si>
+  <si>
+    <t>Assert.AreNotEqual(stack,list);</t>
+  </si>
+  <si>
+    <t>var stack = string.Join(".",deck.SetOfCards);</t>
+  </si>
+  <si>
+    <t>var list = string.Join(".", deck.cards);</t>
+  </si>
+  <si>
+    <t>FALSE Pass</t>
+  </si>
+  <si>
+    <t>F21</t>
+  </si>
+  <si>
+    <t>StartOfRound</t>
+  </si>
+  <si>
+    <t>Assert.AreEqual(dealer.Hand.Count, 2);</t>
+  </si>
+  <si>
+    <t>Kör igenom StartOfRound metoden och tittar så att dealern har fått rätt antal kort i handen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="&quot;docs-Calibri&quot;"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -247,16 +309,18 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="10">
+    <border/>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -265,50 +329,28 @@
       <right style="thin">
         <color rgb="FF999999"/>
       </right>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF999999"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF999999"/>
       </left>
-      <right/>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
       <top style="thin">
         <color rgb="FF999999"/>
       </top>
       <bottom style="thin">
         <color rgb="FF999999"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -317,33 +359,31 @@
       <right style="thin">
         <color rgb="FF999999"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF999999"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF999999"/>
       </left>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF999999"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FF999999"/>
       </right>
       <top style="thin">
         <color rgb="FF999999"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -355,440 +395,141 @@
       <top style="thin">
         <color rgb="FF999999"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF999999"/>
       </left>
-      <right/>
       <top style="thin">
         <color rgb="FF999999"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+  <cellXfs count="16">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF999999"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF999999"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF999999"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF999999"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF999999"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF999999"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF999999"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF999999"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF999999"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF999999"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF999999"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FFD8D8D8"/>
+        </patternFill>
+      </fill>
+      <border/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF999999"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF999999"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF999999"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF999999"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF999999"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF999999"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF999999"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF999999"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF999999"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF999999"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF999999"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF999999"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF999999"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF999999"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF999999"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF999999"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF999999"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF999999"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF999999"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF999999"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF999999"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF999999"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF999999"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF999999"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF999999"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF999999"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDEEAF6"/>
+          <bgColor rgb="FFDEEAF6"/>
+        </patternFill>
+      </fill>
+      <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="1">
+    <tableStyle count="3" pivot="0" name="Blad1-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C365CD27-DED0-4BCB-8F9C-3BA7354AF366}" name="Table1" displayName="Table1" ref="A1:H26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
-  <autoFilter ref="A1:H26" xr:uid="{E93033CE-BFE7-44D2-8C5D-02FF1F3EFF4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H26" displayName="Table_1" id="1">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0A2024A0-3362-4B6A-8F17-486E9F487152}" name="Scenario" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{01F1AA0E-73A2-4D6A-B981-6384E62C7F85}" name="Cases" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{793E7F07-D941-4914-A473-A1D4EBF03601}" name="ID" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4FD93DED-5630-472D-9939-957CC55D5DC4}" name="Steps" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{B3D21B56-6331-4C7A-9682-9E2BD94AE016}" name="Data" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{3BF138EB-AC0D-4114-B7CF-56EA3AAC9B44}" name="Expected" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{F4AB2CC1-2706-4790-ABA7-E33B1E5FFF67}" name="Actual" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{7DFD0621-A157-42ED-A951-4DD7CBFEBEC5}" name="Resualt" dataDxfId="0"/>
+    <tableColumn name="Scenario" id="1"/>
+    <tableColumn name="Cases" id="2"/>
+    <tableColumn name="ID" id="3"/>
+    <tableColumn name="Steps" id="4"/>
+    <tableColumn name="Data" id="5"/>
+    <tableColumn name="Expected" id="6"/>
+    <tableColumn name="Actual" id="7"/>
+    <tableColumn name="Resualt" id="8"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Blad1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -978,501 +719,566 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1001"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
-    <col min="2" max="2" width="32.125" customWidth="1"/>
-    <col min="3" max="3" width="5.25" customWidth="1"/>
-    <col min="4" max="4" width="13.625" customWidth="1"/>
-    <col min="5" max="5" width="17.375" customWidth="1"/>
-    <col min="6" max="7" width="16.25" customWidth="1"/>
-    <col min="8" max="8" width="8.5" customWidth="1"/>
-    <col min="9" max="26" width="7.625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="13.13"/>
+    <col customWidth="1" min="2" max="2" width="32.13"/>
+    <col customWidth="1" min="3" max="3" width="5.25"/>
+    <col customWidth="1" min="4" max="4" width="13.63"/>
+    <col customWidth="1" min="5" max="5" width="17.38"/>
+    <col customWidth="1" min="6" max="7" width="16.25"/>
+    <col customWidth="1" min="8" max="8" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="9" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="33" customHeight="1">
-      <c r="A2" s="6" t="s">
+    <row r="2" ht="33.0" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="b">
+      <c r="F2" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="1" t="b">
+      <c r="G2" s="6" t="b">
         <v>0</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30">
-      <c r="A3" s="6"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="1" t="s">
+    <row r="3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="b">
+      <c r="F3" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="b">
+      <c r="G3" s="6" t="b">
         <v>0</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30">
-      <c r="A4" s="6"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="1" t="s">
+    <row r="4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="b">
+      <c r="F4" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="b">
+      <c r="G4" s="6" t="b">
         <v>1</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="42.75">
-      <c r="A5" s="6"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="1" t="s">
+    <row r="5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="57">
-      <c r="A6" s="6"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
+    <row r="6">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="4" t="b">
+      <c r="F6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="4" t="b">
+      <c r="G6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="47.25" customHeight="1">
-      <c r="A7" s="6" t="s">
+    <row r="7" ht="47.25" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="1" t="b">
+      <c r="F7" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="G7" s="1" t="b">
+      <c r="G7" s="6" t="b">
         <v>0</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="s">
+    <row r="8">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="10" t="s">
         <v>36</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
+    <row r="9">
+      <c r="A9" s="4"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.5">
-      <c r="A10" s="6"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
+    <row r="10">
+      <c r="A10" s="4"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="4" t="b">
+      <c r="F10" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="4" t="b">
+      <c r="G10" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="42.75">
-      <c r="A11" s="6"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4" t="s">
+    <row r="11">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="4" t="b">
+      <c r="F11" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G11" s="4" t="b">
+      <c r="G11" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="57">
-      <c r="A12" s="6"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4" t="s">
+    <row r="12">
+      <c r="A12" s="4"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="28.5">
-      <c r="A13" s="6"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
+    <row r="13">
+      <c r="A13" s="4"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="4" t="b">
+      <c r="G13" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="42.75">
-      <c r="A14" s="6"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4" t="s">
+    <row r="14">
+      <c r="A14" s="4"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="4" t="b">
+      <c r="F14" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G14" s="4" t="b">
+      <c r="G14" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.5">
-      <c r="A15" s="6"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4" t="s">
+    <row r="15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="4" t="b">
+      <c r="F15" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G15" s="4" t="b">
+      <c r="G15" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="57">
-      <c r="A16" s="6"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4" t="s">
+    <row r="16">
+      <c r="A16" s="4"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="6"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="6"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="6"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="6"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="6"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A22" s="6"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+    <row r="17">
+      <c r="A17" s="4"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="4"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="4"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A24" s="6"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="4"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A25" s="6"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="4"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="14"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2441,12 +2247,13 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>